<commit_message>
Nearest neighbourhood search + farthest addition algorithm
</commit_message>
<xml_diff>
--- a/Instances/Coordinates.xlsx
+++ b/Instances/Coordinates.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/07ed5a09c14e9223/BEP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5994F842-6FEE-4382-B084-47FDEF09491B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="8_{5994F842-6FEE-4382-B084-47FDEF09491B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F007A69-4D15-4D9B-9EFA-8D5926F477C7}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D5F24967-34C0-4155-86D0-B197E898762E}"/>
+    <workbookView xWindow="3722" yWindow="3722" windowWidth="19563" windowHeight="10162" xr2:uid="{D5F24967-34C0-4155-86D0-B197E898762E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Blad1" sheetId="1" r:id="rId1"/>
+    <sheet name="c" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,9 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,66 +36,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>Terminal</t>
+    <t>t</t>
   </si>
   <si>
-    <t>X</t>
+    <t>x</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>11.84</t>
-  </si>
-  <si>
-    <t>18.45</t>
-  </si>
-  <si>
-    <t>18.66</t>
-  </si>
-  <si>
-    <t>1.86</t>
-  </si>
-  <si>
-    <t>47.35</t>
-  </si>
-  <si>
-    <t>min 52.49</t>
-  </si>
-  <si>
-    <t>180.76</t>
-  </si>
-  <si>
-    <t>min 73.15</t>
-  </si>
-  <si>
-    <t>240.73</t>
-  </si>
-  <si>
-    <t>min 47.55</t>
-  </si>
-  <si>
-    <t>32.81</t>
-  </si>
-  <si>
-    <t>min 146.37</t>
-  </si>
-  <si>
-    <t>min 104.13</t>
-  </si>
-  <si>
-    <t>273.41</t>
-  </si>
-  <si>
-    <t>min 9.34</t>
-  </si>
-  <si>
-    <t>488.7</t>
-  </si>
-  <si>
-    <t>min 285.08</t>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -132,7 +84,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -148,7 +100,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -444,136 +396,137 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80F722CC-B3AC-48E0-B2C3-8273E0CB1EF1}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B3">
+        <v>11.84</v>
+      </c>
+      <c r="C3">
+        <v>318.45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B4">
+        <v>18.66</v>
+      </c>
+      <c r="C4">
+        <v>301.86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
+      <c r="B5">
+        <v>47.35</v>
+      </c>
+      <c r="C5">
+        <v>247.51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B6">
+        <v>180.76</v>
+      </c>
+      <c r="C6">
+        <v>226.85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>5</v>
       </c>
-      <c r="D4" t="s">
+      <c r="B7">
+        <v>240.73</v>
+      </c>
+      <c r="C7">
+        <v>252.45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B8">
+        <v>32.81</v>
+      </c>
+      <c r="C8">
+        <v>153.63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>7</v>
       </c>
-      <c r="D5" t="s">
+      <c r="B9">
+        <v>240.73</v>
+      </c>
+      <c r="C9">
+        <v>195.87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B10">
+        <v>273.41000000000003</v>
+      </c>
+      <c r="C10">
+        <v>290.66000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>9</v>
       </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="C10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" t="s">
-        <v>19</v>
+      <c r="B11">
+        <v>488.7</v>
+      </c>
+      <c r="C11">
+        <v>14.92</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>